<commit_message>
imp: arreglar cambiar clave por id
</commit_message>
<xml_diff>
--- a/Datasets/Demanda.xlsx
+++ b/Datasets/Demanda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Markdown\Densurbam\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D4A9D-C75D-4DAD-BD52-2B4911C44818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7BBFFD-22EE-48B4-B4D1-F86CF58A1134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>CLAVE_BARRIO</t>
-  </si>
-  <si>
     <t>NOMBRE_BARRIO</t>
   </si>
   <si>
@@ -104,13 +101,16 @@
     <t>AGUA_TODOS_USOS_(L/HAB/AÑO)</t>
   </si>
   <si>
-    <t>CLAVE_MUNICIPIO</t>
-  </si>
-  <si>
-    <t>CLAVE_SECTOR</t>
-  </si>
-  <si>
-    <t>CLAVE_CORREGIMIENTO</t>
+    <t>ID_MUNICIPIO</t>
+  </si>
+  <si>
+    <t>ID_SECTOR</t>
+  </si>
+  <si>
+    <t>ID_CORREGIMIENTO</t>
+  </si>
+  <si>
+    <t>ID_BARRIO</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,25 +483,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -512,7 +512,7 @@
         <v>8371001012</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2">
         <v>837</v>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2">
         <v>68</v>
@@ -539,7 +539,7 @@
         <v>8371008011</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>837</v>
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2">
         <v>68</v>
@@ -566,7 +566,7 @@
         <v>8371008002</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>837</v>
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2">
         <v>68</v>
@@ -593,7 +593,7 @@
         <v>8371006008</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>837</v>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2">
         <v>68</v>
@@ -620,7 +620,7 @@
         <v>8371001024</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>837</v>
@@ -629,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2">
         <v>68</v>
@@ -647,7 +647,7 @@
         <v>8371001010</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>837</v>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2">
         <v>68</v>
@@ -674,7 +674,7 @@
         <v>8371001019</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2">
         <v>837</v>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2">
         <v>68</v>
@@ -701,7 +701,7 @@
         <v>8371008005</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2">
         <v>837</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="2">
         <v>68</v>
@@ -728,7 +728,7 @@
         <v>8371001015</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2">
         <v>837</v>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2">
         <v>68</v>
@@ -755,7 +755,7 @@
         <v>8371001013</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2">
         <v>837</v>
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="2">
         <v>68</v>
@@ -782,7 +782,7 @@
         <v>8371001002</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2">
         <v>837</v>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2">
         <v>68</v>
@@ -809,7 +809,7 @@
         <v>8371001005</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2">
         <v>837</v>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2">
         <v>68</v>
@@ -836,7 +836,7 @@
         <v>8371001001</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2">
         <v>837</v>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="2">
         <v>68</v>
@@ -863,7 +863,7 @@
         <v>8371008003</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2">
         <v>837</v>
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="2">
         <v>68</v>
@@ -890,16 +890,16 @@
         <v>8371001023</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2">
+        <v>837</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D16" s="2">
-        <v>837</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="G16" s="2">
         <v>68</v>

</xml_diff>